<commit_message>
Version 1.1.1; Impressum erstellt
</commit_message>
<xml_diff>
--- a/Allgemeines/Gantt-Projektplan.xlsx
+++ b/Allgemeines/Gantt-Projektplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Finn/Documents/GitHub/APRG_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Finn/Documents/GitHub/APRG_Project/Allgemeines/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Projektplaner</t>
   </si>
@@ -226,12 +226,18 @@
   <si>
     <t>angepasst werden</t>
   </si>
+  <si>
+    <t>Design fehlt</t>
+  </si>
+  <si>
+    <t>Am Wochenende Logik erstellt, Design fehlt noch; eventuell ejs statt html?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -349,6 +355,12 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -590,7 +602,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,6 +681,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -693,6 +717,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -717,20 +744,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -762,7 +777,35 @@
     <cellStyle name="Überschriften für Zeiträume" xfId="3"/>
     <cellStyle name="Zeitraumwert" xfId="13"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -777,6 +820,91 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
         </bottom>
         <vertical/>
@@ -790,6 +918,119 @@
         </top>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1149,10 +1390,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ17"/>
+  <dimension ref="A1:BQ18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1410,7 @@
     <col min="29" max="68" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:43" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1181,14 +1422,14 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:69" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:43" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1198,69 +1439,69 @@
         <v>1</v>
       </c>
       <c r="K2" s="14"/>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="36"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="34" t="s">
+      <c r="R2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="36"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="41"/>
       <c r="V2" s="16"/>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="38"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="43"/>
       <c r="AA2" s="17"/>
-      <c r="AB2" s="39" t="s">
+      <c r="AB2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="41"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="46"/>
       <c r="AI2" s="18"/>
-      <c r="AJ2" s="26" t="s">
+      <c r="AJ2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
     </row>
-    <row r="3" spans="1:69" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="26" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="19" t="s">
@@ -1286,13 +1527,13 @@
       <c r="AA3" s="9"/>
       <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="43"/>
+    <row r="4" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="21"/>
       <c r="H4" s="20" t="s">
         <v>33</v>
@@ -1330,7 +1571,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1342,8 +1583,8 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="28" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="23"/>
@@ -1362,7 +1603,7 @@
       <c r="AA5"/>
       <c r="AB5"/>
     </row>
-    <row r="6" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1375,7 +1616,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="23"/>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="29" t="s">
         <v>36</v>
       </c>
       <c r="H6" s="23"/>
@@ -1394,7 +1635,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -1426,16 +1667,12 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>4</v>
-      </c>
+    <row r="8" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="23"/>
@@ -1456,15 +1693,15 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1486,15 +1723,15 @@
       <c r="AA9"/>
       <c r="AB9"/>
     </row>
-    <row r="10" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
       </c>
       <c r="C10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1516,9 +1753,9 @@
       <c r="AA10"/>
       <c r="AB10"/>
     </row>
-    <row r="11" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
@@ -1529,7 +1766,9 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="22"/>
+      <c r="G11" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="H11" s="23"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -1546,7 +1785,7 @@
       <c r="AA11"/>
       <c r="AB11"/>
     </row>
-    <row r="12" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
@@ -1576,7 +1815,7 @@
       <c r="AA12"/>
       <c r="AB12"/>
     </row>
-    <row r="13" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1606,15 +1845,15 @@
       <c r="AA13"/>
       <c r="AB13"/>
     </row>
-    <row r="14" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
       </c>
       <c r="C14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1636,15 +1875,15 @@
       <c r="AA14"/>
       <c r="AB14"/>
     </row>
-    <row r="15" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1666,94 +1905,66 @@
       <c r="AA15"/>
       <c r="AB15"/>
     </row>
-    <row r="16" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="23"/>
       <c r="G16" s="22"/>
       <c r="H16" s="23"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="25"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="25"/>
-      <c r="Z16" s="25"/>
-      <c r="AA16" s="25"/>
-      <c r="AB16" s="25"/>
-      <c r="AC16" s="25"/>
-      <c r="AD16" s="25"/>
-      <c r="AE16" s="25"/>
-      <c r="AF16" s="25"/>
-      <c r="AG16" s="25"/>
-      <c r="AH16" s="25"/>
-      <c r="AI16" s="25"/>
-      <c r="AJ16" s="25"/>
-      <c r="AK16" s="25"/>
-      <c r="AL16" s="25"/>
-      <c r="AM16" s="25"/>
-      <c r="AN16" s="25"/>
-      <c r="AO16" s="25"/>
-      <c r="AP16" s="25"/>
-      <c r="AQ16" s="25"/>
-      <c r="AR16" s="25"/>
-      <c r="AS16" s="25"/>
-      <c r="AT16" s="25"/>
-      <c r="AU16" s="25"/>
-      <c r="AV16" s="25"/>
-      <c r="AW16" s="25"/>
-      <c r="AX16" s="25"/>
-      <c r="AY16" s="25"/>
-      <c r="AZ16" s="25"/>
-      <c r="BA16" s="25"/>
-      <c r="BB16" s="25"/>
-      <c r="BC16" s="25"/>
-      <c r="BD16" s="25"/>
-      <c r="BE16" s="25"/>
-      <c r="BF16" s="25"/>
-      <c r="BG16" s="25"/>
-      <c r="BH16" s="25"/>
-      <c r="BI16" s="25"/>
-      <c r="BJ16" s="25"/>
-      <c r="BK16" s="25"/>
-      <c r="BL16" s="25"/>
-      <c r="BM16" s="25"/>
-      <c r="BN16" s="25"/>
-      <c r="BO16" s="25"/>
-      <c r="BP16" s="25"/>
-      <c r="BQ16" s="25"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
     </row>
-    <row r="17" spans="14:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
       <c r="AC17" s="25"/>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
@@ -1796,6 +2007,64 @@
       <c r="BP17" s="25"/>
       <c r="BQ17" s="25"/>
     </row>
+    <row r="18" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="25"/>
+      <c r="AD18" s="25"/>
+      <c r="AE18" s="25"/>
+      <c r="AF18" s="25"/>
+      <c r="AG18" s="25"/>
+      <c r="AH18" s="25"/>
+      <c r="AI18" s="25"/>
+      <c r="AJ18" s="25"/>
+      <c r="AK18" s="25"/>
+      <c r="AL18" s="25"/>
+      <c r="AM18" s="25"/>
+      <c r="AN18" s="25"/>
+      <c r="AO18" s="25"/>
+      <c r="AP18" s="25"/>
+      <c r="AQ18" s="25"/>
+      <c r="AR18" s="25"/>
+      <c r="AS18" s="25"/>
+      <c r="AT18" s="25"/>
+      <c r="AU18" s="25"/>
+      <c r="AV18" s="25"/>
+      <c r="AW18" s="25"/>
+      <c r="AX18" s="25"/>
+      <c r="AY18" s="25"/>
+      <c r="AZ18" s="25"/>
+      <c r="BA18" s="25"/>
+      <c r="BB18" s="25"/>
+      <c r="BC18" s="25"/>
+      <c r="BD18" s="25"/>
+      <c r="BE18" s="25"/>
+      <c r="BF18" s="25"/>
+      <c r="BG18" s="25"/>
+      <c r="BH18" s="25"/>
+      <c r="BI18" s="25"/>
+      <c r="BJ18" s="25"/>
+      <c r="BK18" s="25"/>
+      <c r="BL18" s="25"/>
+      <c r="BM18" s="25"/>
+      <c r="BN18" s="25"/>
+      <c r="BO18" s="25"/>
+      <c r="BP18" s="25"/>
+      <c r="BQ18" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="AJ2:AQ2"/>
@@ -1811,40 +2080,66 @@
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AB2:AH2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:N16">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="I5:N9 I11:N17">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>ProzentAbgeschlossenHinter</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>Tatsächlich</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>TatsächlichHinter</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>I$4=Zeitraum_ausgewählt</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:BP17">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A18:BP18">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:N4">
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>I$4=Zeitraum_ausgewählt</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:N10">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>ProzentAbgeschlossen</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>ProzentAbgeschlossenHinter</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Tatsächlich</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>TatsächlichHinter</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>I$4=Zeitraum_ausgewählt</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>I$4=Zeitraum_ausgewählt</formula>
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="15">

</xml_diff>

<commit_message>
Probleme mit Canvas; In ground.ejs soll das Zeichnen möglich sein
</commit_message>
<xml_diff>
--- a/Allgemeines/Gantt-Projektplan.xlsx
+++ b/Allgemeines/Gantt-Projektplan.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Projektplaner</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Am Wochenende Logik erstellt, Design fehlt noch; eventuell ejs statt html?</t>
+  </si>
+  <si>
+    <t>Im Zeitplan (ohne Design, nur Logik):</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,6 +749,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -1277,10 +1283,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ18"/>
+  <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1953,6 +1959,37 @@
       <c r="BO18" s="25"/>
       <c r="BP18" s="25"/>
       <c r="BQ18" s="25"/>
+    </row>
+    <row r="19" spans="1:69" ht="26" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Gant Projektplan final aktualisiert
</commit_message>
<xml_diff>
--- a/Allgemeines/Gantt-Projektplan.xlsx
+++ b/Allgemeines/Gantt-Projektplan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Projektplaner</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Design</t>
   </si>
   <si>
-    <t>Kalenderfunktion</t>
-  </si>
-  <si>
     <t>20.10-22.10</t>
   </si>
   <si>
@@ -228,12 +225,6 @@
   </si>
   <si>
     <t>Design fehlt</t>
-  </si>
-  <si>
-    <t>Am Wochenende Logik erstellt, Design fehlt noch; eventuell ejs statt html?</t>
-  </si>
-  <si>
-    <t>Im Zeitplan (ohne Design, nur Logik):</t>
   </si>
 </sst>
 </file>
@@ -360,13 +351,14 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Corbel"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,8 +400,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor rgb="FF735773"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -523,8 +520,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -604,8 +616,20 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,9 +720,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -750,23 +771,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="% abgeschlossen" xfId="16"/>
     <cellStyle name="Aktivität" xfId="2"/>
     <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Bezeichnung" xfId="5"/>
     <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15"/>
     <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18"/>
     <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17"/>
@@ -1283,10 +1308,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ25"/>
+  <dimension ref="A1:BQ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1328,7 @@
     <col min="29" max="68" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:69" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1315,14 +1340,14 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:43" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:69" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1332,70 +1357,70 @@
         <v>1</v>
       </c>
       <c r="K2" s="14"/>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="41"/>
       <c r="V2" s="16"/>
-      <c r="W2" s="31" t="s">
+      <c r="W2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="44"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="43"/>
       <c r="AA2" s="17"/>
-      <c r="AB2" s="45" t="s">
+      <c r="AB2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="46"/>
-      <c r="AH2" s="47"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="46"/>
       <c r="AI2" s="18"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
     </row>
-    <row r="3" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:69" s="10" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>9</v>
@@ -1420,16 +1445,16 @@
       <c r="AA3" s="9"/>
       <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="39"/>
+    <row r="4" spans="1:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="21"/>
       <c r="H4" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>15</v>
@@ -1464,7 +1489,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:43" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1503,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="27"/>
       <c r="G5" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="14"/>
       <c r="O5"/>
@@ -1496,7 +1521,7 @@
       <c r="AA5"/>
       <c r="AB5"/>
     </row>
-    <row r="6" spans="1:43" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1510,7 +1535,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="23"/>
       <c r="G6" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="14"/>
       <c r="O6"/>
@@ -1528,7 +1553,7 @@
       <c r="AA6"/>
       <c r="AB6"/>
     </row>
-    <row r="7" spans="1:43" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
@@ -1542,7 +1567,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="23"/>
       <c r="G7" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="14"/>
       <c r="O7"/>
@@ -1560,17 +1585,22 @@
       <c r="AA7"/>
       <c r="AB7"/>
     </row>
-    <row r="8" spans="1:43" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+    <row r="8" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="23"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23"/>
+      <c r="N8" s="14"/>
       <c r="O8"/>
       <c r="P8"/>
       <c r="Q8"/>
@@ -1586,21 +1616,22 @@
       <c r="AA8"/>
       <c r="AB8"/>
     </row>
-    <row r="9" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="23"/>
       <c r="G9" s="22"/>
       <c r="H9" s="23"/>
+      <c r="N9" s="14"/>
       <c r="O9"/>
       <c r="P9"/>
       <c r="Q9"/>
@@ -1616,21 +1647,23 @@
       <c r="AA9"/>
       <c r="AB9"/>
     </row>
-    <row r="10" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
       </c>
       <c r="C10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
+      <c r="G10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="14"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
@@ -1646,23 +1679,22 @@
       <c r="AA10"/>
       <c r="AB10"/>
     </row>
-    <row r="11" spans="1:43" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="14"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="M11" s="47"/>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
@@ -1678,9 +1710,9 @@
       <c r="AA11"/>
       <c r="AB11"/>
     </row>
-    <row r="12" spans="1:43" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="7">
         <v>2</v>
@@ -1693,6 +1725,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23"/>
+      <c r="M12" s="47"/>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
@@ -1708,21 +1741,23 @@
       <c r="AA12"/>
       <c r="AB12"/>
     </row>
-    <row r="13" spans="1:43" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="23"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23"/>
+      <c r="J13" s="14"/>
+      <c r="N13" s="47"/>
       <c r="O13"/>
       <c r="P13"/>
       <c r="Q13"/>
@@ -1738,9 +1773,9 @@
       <c r="AA13"/>
       <c r="AB13"/>
     </row>
-    <row r="14" spans="1:43" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B14" s="7">
         <v>3</v>
@@ -1769,22 +1804,22 @@
       <c r="AA14"/>
       <c r="AB14"/>
     </row>
-    <row r="15" spans="1:43" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="23"/>
       <c r="G15" s="22"/>
       <c r="H15" s="23"/>
-      <c r="J15" s="14"/>
+      <c r="N15" s="47"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
@@ -1800,197 +1835,65 @@
       <c r="AA15"/>
       <c r="AB15"/>
     </row>
-    <row r="16" spans="1:43" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="7">
-        <v>3</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="23"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
+    <row r="16" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="25"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+      <c r="AG16" s="25"/>
+      <c r="AH16" s="25"/>
+      <c r="AI16" s="25"/>
+      <c r="AJ16" s="25"/>
+      <c r="AK16" s="25"/>
+      <c r="AL16" s="25"/>
+      <c r="AM16" s="25"/>
+      <c r="AN16" s="25"/>
+      <c r="AO16" s="25"/>
+      <c r="AP16" s="25"/>
+      <c r="AQ16" s="25"/>
+      <c r="AR16" s="25"/>
+      <c r="AS16" s="25"/>
+      <c r="AT16" s="25"/>
+      <c r="AU16" s="25"/>
+      <c r="AV16" s="25"/>
+      <c r="AW16" s="25"/>
+      <c r="AX16" s="25"/>
+      <c r="AY16" s="25"/>
+      <c r="AZ16" s="25"/>
+      <c r="BA16" s="25"/>
+      <c r="BB16" s="25"/>
+      <c r="BC16" s="25"/>
+      <c r="BD16" s="25"/>
+      <c r="BE16" s="25"/>
+      <c r="BF16" s="25"/>
+      <c r="BG16" s="25"/>
+      <c r="BH16" s="25"/>
+      <c r="BI16" s="25"/>
+      <c r="BJ16" s="25"/>
+      <c r="BK16" s="25"/>
+      <c r="BL16" s="25"/>
+      <c r="BM16" s="25"/>
+      <c r="BN16" s="25"/>
+      <c r="BO16" s="25"/>
+      <c r="BP16" s="25"/>
+      <c r="BQ16" s="25"/>
     </row>
-    <row r="17" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="7">
-        <v>4</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="25"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
-      <c r="AD17" s="25"/>
-      <c r="AE17" s="25"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
-      <c r="AH17" s="25"/>
-      <c r="AI17" s="25"/>
-      <c r="AJ17" s="25"/>
-      <c r="AK17" s="25"/>
-      <c r="AL17" s="25"/>
-      <c r="AM17" s="25"/>
-      <c r="AN17" s="25"/>
-      <c r="AO17" s="25"/>
-      <c r="AP17" s="25"/>
-      <c r="AQ17" s="25"/>
-      <c r="AR17" s="25"/>
-      <c r="AS17" s="25"/>
-      <c r="AT17" s="25"/>
-      <c r="AU17" s="25"/>
-      <c r="AV17" s="25"/>
-      <c r="AW17" s="25"/>
-      <c r="AX17" s="25"/>
-      <c r="AY17" s="25"/>
-      <c r="AZ17" s="25"/>
-      <c r="BA17" s="25"/>
-      <c r="BB17" s="25"/>
-      <c r="BC17" s="25"/>
-      <c r="BD17" s="25"/>
-      <c r="BE17" s="25"/>
-      <c r="BF17" s="25"/>
-      <c r="BG17" s="25"/>
-      <c r="BH17" s="25"/>
-      <c r="BI17" s="25"/>
-      <c r="BJ17" s="25"/>
-      <c r="BK17" s="25"/>
-      <c r="BL17" s="25"/>
-      <c r="BM17" s="25"/>
-      <c r="BN17" s="25"/>
-      <c r="BO17" s="25"/>
-      <c r="BP17" s="25"/>
-      <c r="BQ17" s="25"/>
-    </row>
-    <row r="18" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="25"/>
-      <c r="AD18" s="25"/>
-      <c r="AE18" s="25"/>
-      <c r="AF18" s="25"/>
-      <c r="AG18" s="25"/>
-      <c r="AH18" s="25"/>
-      <c r="AI18" s="25"/>
-      <c r="AJ18" s="25"/>
-      <c r="AK18" s="25"/>
-      <c r="AL18" s="25"/>
-      <c r="AM18" s="25"/>
-      <c r="AN18" s="25"/>
-      <c r="AO18" s="25"/>
-      <c r="AP18" s="25"/>
-      <c r="AQ18" s="25"/>
-      <c r="AR18" s="25"/>
-      <c r="AS18" s="25"/>
-      <c r="AT18" s="25"/>
-      <c r="AU18" s="25"/>
-      <c r="AV18" s="25"/>
-      <c r="AW18" s="25"/>
-      <c r="AX18" s="25"/>
-      <c r="AY18" s="25"/>
-      <c r="AZ18" s="25"/>
-      <c r="BA18" s="25"/>
-      <c r="BB18" s="25"/>
-      <c r="BC18" s="25"/>
-      <c r="BD18" s="25"/>
-      <c r="BE18" s="25"/>
-      <c r="BF18" s="25"/>
-      <c r="BG18" s="25"/>
-      <c r="BH18" s="25"/>
-      <c r="BI18" s="25"/>
-      <c r="BJ18" s="25"/>
-      <c r="BK18" s="25"/>
-      <c r="BL18" s="25"/>
-      <c r="BM18" s="25"/>
-      <c r="BN18" s="25"/>
-      <c r="BO18" s="25"/>
-      <c r="BP18" s="25"/>
-      <c r="BQ18" s="25"/>
-    </row>
-    <row r="19" spans="1:69" ht="26" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:69" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="17" ht="26" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="AJ2:AQ2"/>
@@ -2006,7 +1909,7 @@
     <mergeCell ref="W2:Z2"/>
     <mergeCell ref="AB2:AH2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:N9 I11:N13 I16:N17 I14:I15 K14:N15">
+  <conditionalFormatting sqref="I5:N7 I10:N10 I13:I14 K14:N14 I8:M8 I11:L12 N11:N12 K13:M13 I15:M15">
     <cfRule type="expression" dxfId="17" priority="9">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
@@ -2032,7 +1935,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:BP18">
+  <conditionalFormatting sqref="A16:BP16">
     <cfRule type="expression" dxfId="9" priority="10">
       <formula>TRUE</formula>
     </cfRule>
@@ -2042,7 +1945,7 @@
       <formula>I$4=Zeitraum_ausgewählt</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:N10">
+  <conditionalFormatting sqref="I9:M9">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>ProzentAbgeschlossen</formula>
     </cfRule>
@@ -2072,7 +1975,7 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Geben Sie einen Wert von 1 bis 60 ein, oder wählen Sie in der Liste einen Zeitraum aus – drücken Sie ABBRECHEN, ALT+NACH-UNTEN und dann die EINGABETASTE, um einen Wert auszuwählen" prompt="Geben Sie einen Zeitraum im Bereich von 1 bis 60 ein, oder wählen Sie einen Zeitraum in der Liste aus. Drücken Sie ALT+NACH-UNTEN, um in der Liste zu navigieren, und dann EINGABE, um einen Wert auszuwählen." sqref="I2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="K2 H5:H7 H11 J14:J15"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="K2 H5:H7 H10 J13:J14 N8:N9"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer an" sqref="Q2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts an" sqref="V2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer über den Plan hinaus an" sqref="AA2"/>

</xml_diff>